<commit_message>
Spreadsheet not closed, commit thsi too
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/Solenoid.xlsx
+++ b/21-Spreads4Tests/Solenoid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154D2B3F-97FB-6243-B5DB-045684F502BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B35ADED-EAEA-004E-8203-7AD480B9D2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="900" windowWidth="23820" windowHeight="15060" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H24" sqref="H24:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1508,21 +1508,21 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" s="23">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="23">
         <f t="array" ref="E24:E27">MMULT(B19:E22,B24:B27)</f>
-        <v>0.22827333781979081</v>
+        <v>2.1647418410607036E-2</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="23">
         <f>B$24*B19+B$25*C19+B$26*D19+B$27*E19</f>
-        <v>0.22827333781979081</v>
+        <v>2.1647418410607036E-2</v>
       </c>
       <c r="K24" s="41">
         <f>E24-H24</f>
@@ -1534,11 +1534,11 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="24">
-        <v>-0.16657258415124282</v>
+        <v>-3.3490533158663523E-2</v>
       </c>
       <c r="H25" s="24">
         <f>B$24*B20+B$25*C20+B$26*D20+B$27*E20</f>
-        <v>-0.16657258415124282</v>
+        <v>-3.3490533158663523E-2</v>
       </c>
       <c r="K25" s="42">
         <f>E25-H25</f>
@@ -1550,14 +1550,14 @@
         <v>6</v>
       </c>
       <c r="B26" s="24">
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="E26" s="24">
-        <v>-0.54739631048262893</v>
+        <v>-0.22388770395486457</v>
       </c>
       <c r="H26" s="24">
         <f>B$24*B21+B$25*C21+B$26*D21+B$27*E21</f>
-        <v>-0.54739631048262893</v>
+        <v>-0.22388770395486457</v>
       </c>
       <c r="K26" s="42">
         <f>E26-H26</f>
@@ -1569,11 +1569,11 @@
         <v>-0.2</v>
       </c>
       <c r="E27" s="25">
-        <v>9.2788839004356083E-2</v>
+        <v>-0.11557412433330472</v>
       </c>
       <c r="H27" s="25">
         <f>B$24*B22+B$25*C22+B$26*D22+B$27*E22</f>
-        <v>9.2788839004356083E-2</v>
+        <v>-0.11557412433330472</v>
       </c>
       <c r="K27" s="43">
         <f>E27-H27</f>

</xml_diff>